<commit_message>
[REF]Agregando reglas salariales mensuales
</commit_message>
<xml_diff>
--- a/data/anticipo.xlsx
+++ b/data/anticipo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\odoo-tool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1434C561-9537-4C9B-BC8F-1BF2EA0B5CA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B59843E-AA07-438B-BB49-D0E6F1F0AF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5328" yWindow="3588" windowWidth="17280" windowHeight="8976" xr2:uid="{C6D3C523-3AAD-4BFA-ABC9-BEC52FFC66BA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C6D3C523-3AAD-4BFA-ABC9-BEC52FFC66BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>HRBPR</t>
   </si>
   <si>
-    <t>HRBCD</t>
-  </si>
-  <si>
     <t>COMIS</t>
   </si>
   <si>
@@ -94,6 +91,9 @@
   </si>
   <si>
     <t>result = HRTIG</t>
+  </si>
+  <si>
+    <t>HRBDC</t>
   </si>
 </sst>
 </file>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE885352-BC20-4EFA-B073-DC55504A8636}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,10 +462,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -484,105 +484,105 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>